<commit_message>
Fixed bug where reader parsed European decimals incorrectly
</commit_message>
<xml_diff>
--- a/LightweightExcelReader.Tests/TestSpreadsheets/Booleans.xlsx
+++ b/LightweightExcelReader.Tests/TestSpreadsheets/Booleans.xlsx
@@ -29,9 +29,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="General"/>
+    <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -103,11 +104,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -134,7 +135,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="n">
@@ -145,7 +146,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- Migrate Tests project to .NET Core - Fix data file of BooleansWork test
</commit_message>
<xml_diff>
--- a/LightweightExcelReader.Tests/TestSpreadsheets/Booleans.xlsx
+++ b/LightweightExcelReader.Tests/TestSpreadsheets/Booleans.xlsx
@@ -132,18 +132,17 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="B1" s="2" t="b">
         <v>0</v>
       </c>
       <c r="K1" s="1" t="s">
@@ -155,18 +154,17 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="B2" s="2" t="b">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normál"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normál"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>